<commit_message>
update: calculate productivity and FLC
</commit_message>
<xml_diff>
--- a/myCode/Ag2050/1_Scripts/output_by_scenario.xlsx
+++ b/myCode/Ag2050/1_Scripts/output_by_scenario.xlsx
@@ -1841,10 +1841,10 @@
         <v>1.004977100045006</v>
       </c>
       <c r="I6" t="n">
-        <v>1.004594820384294</v>
+        <v>0.9959492779147587</v>
       </c>
       <c r="J6" t="n">
-        <v>1.004594820384294</v>
+        <v>0.9959492779147587</v>
       </c>
       <c r="K6" t="n">
         <v>1.010759479266239</v>
@@ -1943,10 +1943,10 @@
         <v>1.005910946632596</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1.004594820384294</v>
+        <v>0.9959492779147587</v>
       </c>
       <c r="AR6" t="n">
-        <v>1.004594820384294</v>
+        <v>0.9959492779147587</v>
       </c>
       <c r="AS6" t="n">
         <v>1.010763689067928</v>
@@ -2050,10 +2050,10 @@
         <v>1.009954200090011</v>
       </c>
       <c r="I7" t="n">
-        <v>1.009189640768588</v>
+        <v>0.9918985558295175</v>
       </c>
       <c r="J7" t="n">
-        <v>1.009189640768588</v>
+        <v>0.9918985558295175</v>
       </c>
       <c r="K7" t="n">
         <v>1.021518958532478</v>
@@ -2152,10 +2152,10 @@
         <v>1.011821893265192</v>
       </c>
       <c r="AQ7" t="n">
-        <v>1.009189640768588</v>
+        <v>0.9918985558295175</v>
       </c>
       <c r="AR7" t="n">
-        <v>1.009189640768588</v>
+        <v>0.9918985558295175</v>
       </c>
       <c r="AS7" t="n">
         <v>1.021527378135857</v>
@@ -2259,10 +2259,10 @@
         <v>1.014931300135017</v>
       </c>
       <c r="I8" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9878478337442762</v>
       </c>
       <c r="J8" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9878478337442762</v>
       </c>
       <c r="K8" t="n">
         <v>1.032278437798716</v>
@@ -2361,10 +2361,10 @@
         <v>1.017732839897788</v>
       </c>
       <c r="AQ8" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9878478337442762</v>
       </c>
       <c r="AR8" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9878478337442762</v>
       </c>
       <c r="AS8" t="n">
         <v>1.032291067203785</v>
@@ -2468,10 +2468,10 @@
         <v>1.019908400180023</v>
       </c>
       <c r="I9" t="n">
-        <v>1.018379281537176</v>
+        <v>0.9837971116590348</v>
       </c>
       <c r="J9" t="n">
-        <v>1.018379281537176</v>
+        <v>0.9837971116590348</v>
       </c>
       <c r="K9" t="n">
         <v>1.043037917064955</v>
@@ -2570,10 +2570,10 @@
         <v>1.023643786530384</v>
       </c>
       <c r="AQ9" t="n">
-        <v>1.018379281537176</v>
+        <v>0.9837971116590348</v>
       </c>
       <c r="AR9" t="n">
-        <v>1.018379281537176</v>
+        <v>0.9837971116590348</v>
       </c>
       <c r="AS9" t="n">
         <v>1.043054756271714</v>
@@ -2677,10 +2677,10 @@
         <v>1.024885500225029</v>
       </c>
       <c r="I10" t="n">
-        <v>1.02297410192147</v>
+        <v>0.9797463895737936</v>
       </c>
       <c r="J10" t="n">
-        <v>1.02297410192147</v>
+        <v>0.9797463895737936</v>
       </c>
       <c r="K10" t="n">
         <v>1.053797396331194</v>
@@ -2779,10 +2779,10 @@
         <v>1.029554733162981</v>
       </c>
       <c r="AQ10" t="n">
-        <v>1.02297410192147</v>
+        <v>0.9797463895737936</v>
       </c>
       <c r="AR10" t="n">
-        <v>1.02297410192147</v>
+        <v>0.9797463895737936</v>
       </c>
       <c r="AS10" t="n">
         <v>1.053818445339642</v>
@@ -2886,10 +2886,10 @@
         <v>1.029862600270034</v>
       </c>
       <c r="I11" t="n">
-        <v>1.027568922305764</v>
+        <v>0.9756956674885523</v>
       </c>
       <c r="J11" t="n">
-        <v>1.027568922305764</v>
+        <v>0.9756956674885523</v>
       </c>
       <c r="K11" t="n">
         <v>1.064556875597433</v>
@@ -2988,10 +2988,10 @@
         <v>1.035465679795577</v>
       </c>
       <c r="AQ11" t="n">
-        <v>1.027568922305764</v>
+        <v>0.9756956674885523</v>
       </c>
       <c r="AR11" t="n">
-        <v>1.027568922305764</v>
+        <v>0.9756956674885523</v>
       </c>
       <c r="AS11" t="n">
         <v>1.064582134407571</v>
@@ -3095,10 +3095,10 @@
         <v>1.03483970031504</v>
       </c>
       <c r="I12" t="n">
-        <v>1.032163742690059</v>
+        <v>0.971644945403311</v>
       </c>
       <c r="J12" t="n">
-        <v>1.032163742690059</v>
+        <v>0.971644945403311</v>
       </c>
       <c r="K12" t="n">
         <v>1.075316354863671</v>
@@ -3197,10 +3197,10 @@
         <v>1.041376626428173</v>
       </c>
       <c r="AQ12" t="n">
-        <v>1.032163742690059</v>
+        <v>0.971644945403311</v>
       </c>
       <c r="AR12" t="n">
-        <v>1.032163742690059</v>
+        <v>0.971644945403311</v>
       </c>
       <c r="AS12" t="n">
         <v>1.075345823475499</v>
@@ -3304,10 +3304,10 @@
         <v>1.039816800360046</v>
       </c>
       <c r="I13" t="n">
-        <v>1.036758563074353</v>
+        <v>0.9675942233180698</v>
       </c>
       <c r="J13" t="n">
-        <v>1.036758563074353</v>
+        <v>0.9675942233180698</v>
       </c>
       <c r="K13" t="n">
         <v>1.08607583412991</v>
@@ -3406,10 +3406,10 @@
         <v>1.047287573060769</v>
       </c>
       <c r="AQ13" t="n">
-        <v>1.036758563074353</v>
+        <v>0.9675942233180698</v>
       </c>
       <c r="AR13" t="n">
-        <v>1.036758563074353</v>
+        <v>0.9675942233180698</v>
       </c>
       <c r="AS13" t="n">
         <v>1.086109512543428</v>
@@ -3513,10 +3513,10 @@
         <v>1.044793900405051</v>
       </c>
       <c r="I14" t="n">
-        <v>1.041353383458647</v>
+        <v>0.9635435012328284</v>
       </c>
       <c r="J14" t="n">
-        <v>1.041353383458647</v>
+        <v>0.9635435012328284</v>
       </c>
       <c r="K14" t="n">
         <v>1.096835313396149</v>
@@ -3615,10 +3615,10 @@
         <v>1.053198519693365</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.041353383458647</v>
+        <v>0.9635435012328284</v>
       </c>
       <c r="AR14" t="n">
-        <v>1.041353383458647</v>
+        <v>0.9635435012328284</v>
       </c>
       <c r="AS14" t="n">
         <v>1.096873201611356</v>
@@ -3722,10 +3722,10 @@
         <v>1.049771000450057</v>
       </c>
       <c r="I15" t="n">
-        <v>1.045948203842941</v>
+        <v>0.9594927791475871</v>
       </c>
       <c r="J15" t="n">
-        <v>1.045948203842941</v>
+        <v>0.9594927791475871</v>
       </c>
       <c r="K15" t="n">
         <v>1.107594792662388</v>
@@ -3824,10 +3824,10 @@
         <v>1.059109466325961</v>
       </c>
       <c r="AQ15" t="n">
-        <v>1.045948203842941</v>
+        <v>0.9594927791475871</v>
       </c>
       <c r="AR15" t="n">
-        <v>1.045948203842941</v>
+        <v>0.9594927791475871</v>
       </c>
       <c r="AS15" t="n">
         <v>1.107636890679285</v>
@@ -3931,10 +3931,10 @@
         <v>1.054748100495063</v>
       </c>
       <c r="I16" t="n">
-        <v>1.050543024227235</v>
+        <v>0.9554420570623459</v>
       </c>
       <c r="J16" t="n">
-        <v>1.050543024227235</v>
+        <v>0.9554420570623459</v>
       </c>
       <c r="K16" t="n">
         <v>1.118354271928627</v>
@@ -4033,10 +4033,10 @@
         <v>1.065020412958557</v>
       </c>
       <c r="AQ16" t="n">
-        <v>1.050543024227235</v>
+        <v>0.9554420570623459</v>
       </c>
       <c r="AR16" t="n">
-        <v>1.050543024227235</v>
+        <v>0.9554420570623459</v>
       </c>
       <c r="AS16" t="n">
         <v>1.118400579747213</v>
@@ -4140,10 +4140,10 @@
         <v>1.059725200540068</v>
       </c>
       <c r="I17" t="n">
-        <v>1.055137844611529</v>
+        <v>0.9513913349771046</v>
       </c>
       <c r="J17" t="n">
-        <v>1.055137844611529</v>
+        <v>0.9513913349771046</v>
       </c>
       <c r="K17" t="n">
         <v>1.129113751194865</v>
@@ -4242,10 +4242,10 @@
         <v>1.070931359591153</v>
       </c>
       <c r="AQ17" t="n">
-        <v>1.055137844611529</v>
+        <v>0.9513913349771046</v>
       </c>
       <c r="AR17" t="n">
-        <v>1.055137844611529</v>
+        <v>0.9513913349771046</v>
       </c>
       <c r="AS17" t="n">
         <v>1.129164268815142</v>
@@ -4349,10 +4349,10 @@
         <v>1.064702300585074</v>
       </c>
       <c r="I18" t="n">
-        <v>1.059732664995823</v>
+        <v>0.9473406128918633</v>
       </c>
       <c r="J18" t="n">
-        <v>1.059732664995823</v>
+        <v>0.9473406128918633</v>
       </c>
       <c r="K18" t="n">
         <v>1.139873230461104</v>
@@ -4451,10 +4451,10 @@
         <v>1.07684230622375</v>
       </c>
       <c r="AQ18" t="n">
-        <v>1.059732664995823</v>
+        <v>0.9473406128918633</v>
       </c>
       <c r="AR18" t="n">
-        <v>1.059732664995823</v>
+        <v>0.9473406128918633</v>
       </c>
       <c r="AS18" t="n">
         <v>1.13992795788307</v>
@@ -4558,10 +4558,10 @@
         <v>1.06967940063008</v>
       </c>
       <c r="I19" t="n">
-        <v>1.064327485380117</v>
+        <v>0.9432898908066221</v>
       </c>
       <c r="J19" t="n">
-        <v>1.064327485380117</v>
+        <v>0.9432898908066221</v>
       </c>
       <c r="K19" t="n">
         <v>1.150632709727343</v>
@@ -4660,10 +4660,10 @@
         <v>1.082753252856346</v>
       </c>
       <c r="AQ19" t="n">
-        <v>1.064327485380117</v>
+        <v>0.9432898908066221</v>
       </c>
       <c r="AR19" t="n">
-        <v>1.064327485380117</v>
+        <v>0.9432898908066221</v>
       </c>
       <c r="AS19" t="n">
         <v>1.150691646950998</v>
@@ -4767,10 +4767,10 @@
         <v>1.074656500675085</v>
       </c>
       <c r="I20" t="n">
-        <v>1.068922305764411</v>
+        <v>0.9392391687213808</v>
       </c>
       <c r="J20" t="n">
-        <v>1.068922305764411</v>
+        <v>0.9392391687213808</v>
       </c>
       <c r="K20" t="n">
         <v>1.161392188993582</v>
@@ -4869,10 +4869,10 @@
         <v>1.088664199488942</v>
       </c>
       <c r="AQ20" t="n">
-        <v>1.068922305764411</v>
+        <v>0.9392391687213808</v>
       </c>
       <c r="AR20" t="n">
-        <v>1.068922305764411</v>
+        <v>0.9392391687213808</v>
       </c>
       <c r="AS20" t="n">
         <v>1.161455336018927</v>
@@ -4976,10 +4976,10 @@
         <v>1.079633600720091</v>
       </c>
       <c r="I21" t="n">
-        <v>1.073517126148705</v>
+        <v>0.9351884466361394</v>
       </c>
       <c r="J21" t="n">
-        <v>1.073517126148705</v>
+        <v>0.9351884466361394</v>
       </c>
       <c r="K21" t="n">
         <v>1.172151668259821</v>
@@ -5078,10 +5078,10 @@
         <v>1.094575146121538</v>
       </c>
       <c r="AQ21" t="n">
-        <v>1.073517126148705</v>
+        <v>0.9351884466361394</v>
       </c>
       <c r="AR21" t="n">
-        <v>1.073517126148705</v>
+        <v>0.9351884466361394</v>
       </c>
       <c r="AS21" t="n">
         <v>1.172219025086855</v>
@@ -5185,10 +5185,10 @@
         <v>1.084610700765097</v>
       </c>
       <c r="I22" t="n">
-        <v>1.078111946532999</v>
+        <v>0.9311377245508982</v>
       </c>
       <c r="J22" t="n">
-        <v>1.078111946532999</v>
+        <v>0.9311377245508982</v>
       </c>
       <c r="K22" t="n">
         <v>1.182911147526059</v>
@@ -5287,10 +5287,10 @@
         <v>1.100486092754134</v>
       </c>
       <c r="AQ22" t="n">
-        <v>1.078111946532999</v>
+        <v>0.9311377245508982</v>
       </c>
       <c r="AR22" t="n">
-        <v>1.078111946532999</v>
+        <v>0.9311377245508982</v>
       </c>
       <c r="AS22" t="n">
         <v>1.182982714154784</v>
@@ -5394,10 +5394,10 @@
         <v>1.089587800810103</v>
       </c>
       <c r="I23" t="n">
-        <v>1.082706766917293</v>
+        <v>0.9270870024656569</v>
       </c>
       <c r="J23" t="n">
-        <v>1.082706766917293</v>
+        <v>0.9270870024656569</v>
       </c>
       <c r="K23" t="n">
         <v>1.193670626792298</v>
@@ -5496,10 +5496,10 @@
         <v>1.10639703938673</v>
       </c>
       <c r="AQ23" t="n">
-        <v>1.082706766917293</v>
+        <v>0.9270870024656569</v>
       </c>
       <c r="AR23" t="n">
-        <v>1.082706766917293</v>
+        <v>0.9270870024656569</v>
       </c>
       <c r="AS23" t="n">
         <v>1.193746403222712</v>
@@ -5603,10 +5603,10 @@
         <v>1.092351679771265</v>
       </c>
       <c r="I24" t="n">
-        <v>1.084962406015038</v>
+        <v>0.9231067277210285</v>
       </c>
       <c r="J24" t="n">
-        <v>1.084962406015038</v>
+        <v>0.9231067277210285</v>
       </c>
       <c r="K24" t="n">
         <v>1.204035231462515</v>
@@ -5705,10 +5705,10 @@
         <v>1.1101506740682</v>
       </c>
       <c r="AQ24" t="n">
-        <v>1.084962406015038</v>
+        <v>0.9231067277210285</v>
       </c>
       <c r="AR24" t="n">
-        <v>1.084962406015038</v>
+        <v>0.9231067277210285</v>
       </c>
       <c r="AS24" t="n">
         <v>1.204105121810857</v>
@@ -5812,10 +5812,10 @@
         <v>1.095115558732428</v>
       </c>
       <c r="I25" t="n">
-        <v>1.087218045112782</v>
+        <v>0.9191264529764002</v>
       </c>
       <c r="J25" t="n">
-        <v>1.087218045112782</v>
+        <v>0.9191264529764002</v>
       </c>
       <c r="K25" t="n">
         <v>1.214399836132733</v>
@@ -5914,10 +5914,10 @@
         <v>1.11390430874967</v>
       </c>
       <c r="AQ25" t="n">
-        <v>1.087218045112782</v>
+        <v>0.9191264529764002</v>
       </c>
       <c r="AR25" t="n">
-        <v>1.087218045112782</v>
+        <v>0.9191264529764002</v>
       </c>
       <c r="AS25" t="n">
         <v>1.214463840399002</v>
@@ -6021,10 +6021,10 @@
         <v>1.097879437693591</v>
       </c>
       <c r="I26" t="n">
-        <v>1.089473684210526</v>
+        <v>0.9151461782317717</v>
       </c>
       <c r="J26" t="n">
-        <v>1.089473684210526</v>
+        <v>0.9151461782317717</v>
       </c>
       <c r="K26" t="n">
         <v>1.22476444080295</v>
@@ -6123,10 +6123,10 @@
         <v>1.117657943431139</v>
       </c>
       <c r="AQ26" t="n">
-        <v>1.089473684210526</v>
+        <v>0.9151461782317717</v>
       </c>
       <c r="AR26" t="n">
-        <v>1.089473684210526</v>
+        <v>0.9151461782317717</v>
       </c>
       <c r="AS26" t="n">
         <v>1.224822558987148</v>
@@ -6230,10 +6230,10 @@
         <v>1.100643316654753</v>
       </c>
       <c r="I27" t="n">
-        <v>1.091729323308271</v>
+        <v>0.9111659034871433</v>
       </c>
       <c r="J27" t="n">
-        <v>1.091729323308271</v>
+        <v>0.9111659034871433</v>
       </c>
       <c r="K27" t="n">
         <v>1.235129045473167</v>
@@ -6332,10 +6332,10 @@
         <v>1.121411578112609</v>
       </c>
       <c r="AQ27" t="n">
-        <v>1.091729323308271</v>
+        <v>0.9111659034871433</v>
       </c>
       <c r="AR27" t="n">
-        <v>1.091729323308271</v>
+        <v>0.9111659034871433</v>
       </c>
       <c r="AS27" t="n">
         <v>1.235181277575293</v>
@@ -6439,10 +6439,10 @@
         <v>1.103407195615916</v>
       </c>
       <c r="I28" t="n">
-        <v>1.093984962406015</v>
+        <v>0.907185628742515</v>
       </c>
       <c r="J28" t="n">
-        <v>1.093984962406015</v>
+        <v>0.907185628742515</v>
       </c>
       <c r="K28" t="n">
         <v>1.245493650143384</v>
@@ -6541,10 +6541,10 @@
         <v>1.125165212794079</v>
       </c>
       <c r="AQ28" t="n">
-        <v>1.093984962406015</v>
+        <v>0.907185628742515</v>
       </c>
       <c r="AR28" t="n">
-        <v>1.093984962406015</v>
+        <v>0.907185628742515</v>
       </c>
       <c r="AS28" t="n">
         <v>1.245539996163438</v>
@@ -6648,10 +6648,10 @@
         <v>1.105599237550631</v>
       </c>
       <c r="I29" t="n">
-        <v>1.096992481203007</v>
+        <v>0.9037689327227897</v>
       </c>
       <c r="J29" t="n">
-        <v>1.096992481203007</v>
+        <v>0.9037689327227897</v>
       </c>
       <c r="K29" t="n">
         <v>1.255858254813601</v>
@@ -6750,10 +6750,10 @@
         <v>1.128363732487444</v>
       </c>
       <c r="AQ29" t="n">
-        <v>1.096992481203007</v>
+        <v>0.9037689327227897</v>
       </c>
       <c r="AR29" t="n">
-        <v>1.096992481203007</v>
+        <v>0.9037689327227897</v>
       </c>
       <c r="AS29" t="n">
         <v>1.255917897563783</v>
@@ -6857,10 +6857,10 @@
         <v>1.107791279485347</v>
       </c>
       <c r="I30" t="n">
-        <v>1.1</v>
+        <v>0.9003522367030644</v>
       </c>
       <c r="J30" t="n">
-        <v>1.1</v>
+        <v>0.9003522367030644</v>
       </c>
       <c r="K30" t="n">
         <v>1.266222859483818</v>
@@ -6959,10 +6959,10 @@
         <v>1.131562252180809</v>
       </c>
       <c r="AQ30" t="n">
-        <v>1.1</v>
+        <v>0.9003522367030644</v>
       </c>
       <c r="AR30" t="n">
-        <v>1.1</v>
+        <v>0.9003522367030644</v>
       </c>
       <c r="AS30" t="n">
         <v>1.266295798964128</v>
@@ -7066,10 +7066,10 @@
         <v>1.109983321420062</v>
       </c>
       <c r="I31" t="n">
-        <v>1.103007518796993</v>
+        <v>0.8969355406833392</v>
       </c>
       <c r="J31" t="n">
-        <v>1.103007518796993</v>
+        <v>0.8969355406833392</v>
       </c>
       <c r="K31" t="n">
         <v>1.276587464154035</v>
@@ -7168,10 +7168,10 @@
         <v>1.134760771874174</v>
       </c>
       <c r="AQ31" t="n">
-        <v>1.103007518796993</v>
+        <v>0.8969355406833392</v>
       </c>
       <c r="AR31" t="n">
-        <v>1.103007518796993</v>
+        <v>0.8969355406833392</v>
       </c>
       <c r="AS31" t="n">
         <v>1.276673700364473</v>
@@ -7275,10 +7275,10 @@
         <v>1.112175363354777</v>
       </c>
       <c r="I32" t="n">
-        <v>1.106015037593985</v>
+        <v>0.893518844663614</v>
       </c>
       <c r="J32" t="n">
-        <v>1.106015037593985</v>
+        <v>0.893518844663614</v>
       </c>
       <c r="K32" t="n">
         <v>1.286952068824252</v>
@@ -7377,10 +7377,10 @@
         <v>1.137959291567539</v>
       </c>
       <c r="AQ32" t="n">
-        <v>1.106015037593985</v>
+        <v>0.893518844663614</v>
       </c>
       <c r="AR32" t="n">
-        <v>1.106015037593985</v>
+        <v>0.893518844663614</v>
       </c>
       <c r="AS32" t="n">
         <v>1.287051601764819</v>
@@ -7484,10 +7484,10 @@
         <v>1.114367405289492</v>
       </c>
       <c r="I33" t="n">
-        <v>1.109022556390977</v>
+        <v>0.8901021486438887</v>
       </c>
       <c r="J33" t="n">
-        <v>1.109022556390977</v>
+        <v>0.8901021486438887</v>
       </c>
       <c r="K33" t="n">
         <v>1.297316673494469</v>
@@ -7586,10 +7586,10 @@
         <v>1.141157811260904</v>
       </c>
       <c r="AQ33" t="n">
-        <v>1.109022556390977</v>
+        <v>0.8901021486438887</v>
       </c>
       <c r="AR33" t="n">
-        <v>1.109022556390977</v>
+        <v>0.8901021486438887</v>
       </c>
       <c r="AS33" t="n">
         <v>1.297429503165164</v>
@@ -7693,10 +7693,10 @@
         <v>1.11582082439838</v>
       </c>
       <c r="I34" t="n">
-        <v>1.11203007518797</v>
+        <v>0.8873899260302923</v>
       </c>
       <c r="J34" t="n">
-        <v>1.11203007518797</v>
+        <v>0.8873899260302923</v>
       </c>
       <c r="K34" t="n">
         <v>1.307230643179025</v>
@@ -7795,10 +7795,10 @@
         <v>1.143629394660323</v>
       </c>
       <c r="AQ34" t="n">
-        <v>1.11203007518797</v>
+        <v>0.8873899260302923</v>
       </c>
       <c r="AR34" t="n">
-        <v>1.11203007518797</v>
+        <v>0.8873899260302923</v>
       </c>
       <c r="AS34" t="n">
         <v>1.307337425666603</v>
@@ -7902,10 +7902,10 @@
         <v>1.117274243507267</v>
       </c>
       <c r="I35" t="n">
-        <v>1.115037593984962</v>
+        <v>0.884677703416696</v>
       </c>
       <c r="J35" t="n">
-        <v>1.115037593984962</v>
+        <v>0.884677703416696</v>
       </c>
       <c r="K35" t="n">
         <v>1.31714461286358</v>
@@ -8004,10 +8004,10 @@
         <v>1.146100978059741</v>
       </c>
       <c r="AQ35" t="n">
-        <v>1.115037593984962</v>
+        <v>0.884677703416696</v>
       </c>
       <c r="AR35" t="n">
-        <v>1.115037593984962</v>
+        <v>0.884677703416696</v>
       </c>
       <c r="AS35" t="n">
         <v>1.317245348168041</v>
@@ -8111,10 +8111,10 @@
         <v>1.118727662616154</v>
       </c>
       <c r="I36" t="n">
-        <v>1.118045112781955</v>
+        <v>0.8819654808030997</v>
       </c>
       <c r="J36" t="n">
-        <v>1.118045112781955</v>
+        <v>0.8819654808030997</v>
       </c>
       <c r="K36" t="n">
         <v>1.327058582548136</v>
@@ -8213,10 +8213,10 @@
         <v>1.14857256145916</v>
       </c>
       <c r="AQ36" t="n">
-        <v>1.118045112781955</v>
+        <v>0.8819654808030997</v>
       </c>
       <c r="AR36" t="n">
-        <v>1.118045112781955</v>
+        <v>0.8819654808030997</v>
       </c>
       <c r="AS36" t="n">
         <v>1.32715327066948</v>
@@ -8320,10 +8320,10 @@
         <v>1.120181081725041</v>
       </c>
       <c r="I37" t="n">
-        <v>1.121052631578947</v>
+        <v>0.8792532581895034</v>
       </c>
       <c r="J37" t="n">
-        <v>1.121052631578947</v>
+        <v>0.8792532581895034</v>
       </c>
       <c r="K37" t="n">
         <v>1.336972552232691</v>
@@ -8422,10 +8422,10 @@
         <v>1.151044144858578</v>
       </c>
       <c r="AQ37" t="n">
-        <v>1.121052631578947</v>
+        <v>0.8792532581895034</v>
       </c>
       <c r="AR37" t="n">
-        <v>1.121052631578947</v>
+        <v>0.8792532581895034</v>
       </c>
       <c r="AS37" t="n">
         <v>1.337061193170919</v>
@@ -8529,10 +8529,10 @@
         <v>1.121634500833929</v>
       </c>
       <c r="I38" t="n">
-        <v>1.12406015037594</v>
+        <v>0.876541035575907</v>
       </c>
       <c r="J38" t="n">
-        <v>1.12406015037594</v>
+        <v>0.876541035575907</v>
       </c>
       <c r="K38" t="n">
         <v>1.346886521917247</v>
@@ -8631,10 +8631,10 @@
         <v>1.153515728257996</v>
       </c>
       <c r="AQ38" t="n">
-        <v>1.12406015037594</v>
+        <v>0.876541035575907</v>
       </c>
       <c r="AR38" t="n">
-        <v>1.12406015037594</v>
+        <v>0.876541035575907</v>
       </c>
       <c r="AS38" t="n">
         <v>1.346969115672358</v>
@@ -8738,10 +8738,10 @@
         <v>1.123087919942816</v>
       </c>
       <c r="I39" t="n">
-        <v>1.127067669172932</v>
+        <v>0.8738288129623106</v>
       </c>
       <c r="J39" t="n">
-        <v>1.127067669172932</v>
+        <v>0.8738288129623106</v>
       </c>
       <c r="K39" t="n">
         <v>1.356800491601803</v>
@@ -8840,10 +8840,10 @@
         <v>1.155987311657415</v>
       </c>
       <c r="AQ39" t="n">
-        <v>1.127067669172932</v>
+        <v>0.8738288129623106</v>
       </c>
       <c r="AR39" t="n">
-        <v>1.127067669172932</v>
+        <v>0.8738288129623106</v>
       </c>
       <c r="AS39" t="n">
         <v>1.356877038173796</v>
@@ -8947,10 +8947,10 @@
         <v>1.124541339051704</v>
       </c>
       <c r="I40" t="n">
-        <v>1.130075187969925</v>
+        <v>0.8711165903487144</v>
       </c>
       <c r="J40" t="n">
-        <v>1.130075187969925</v>
+        <v>0.8711165903487144</v>
       </c>
       <c r="K40" t="n">
         <v>1.366714461286358</v>
@@ -9049,10 +9049,10 @@
         <v>1.158458895056833</v>
       </c>
       <c r="AQ40" t="n">
-        <v>1.130075187969925</v>
+        <v>0.8711165903487144</v>
       </c>
       <c r="AR40" t="n">
-        <v>1.130075187969925</v>
+        <v>0.8711165903487144</v>
       </c>
       <c r="AS40" t="n">
         <v>1.366784960675235</v>
@@ -9156,10 +9156,10 @@
         <v>1.125994758160591</v>
       </c>
       <c r="I41" t="n">
-        <v>1.133082706766917</v>
+        <v>0.868404367735118</v>
       </c>
       <c r="J41" t="n">
-        <v>1.133082706766917</v>
+        <v>0.868404367735118</v>
       </c>
       <c r="K41" t="n">
         <v>1.376628430970914</v>
@@ -9258,10 +9258,10 @@
         <v>1.160930478456252</v>
       </c>
       <c r="AQ41" t="n">
-        <v>1.133082706766917</v>
+        <v>0.868404367735118</v>
       </c>
       <c r="AR41" t="n">
-        <v>1.133082706766917</v>
+        <v>0.868404367735118</v>
       </c>
       <c r="AS41" t="n">
         <v>1.376692883176674</v>
@@ -9365,10 +9365,10 @@
         <v>1.127448177269478</v>
       </c>
       <c r="I42" t="n">
-        <v>1.13609022556391</v>
+        <v>0.8656921451215217</v>
       </c>
       <c r="J42" t="n">
-        <v>1.13609022556391</v>
+        <v>0.8656921451215217</v>
       </c>
       <c r="K42" t="n">
         <v>1.386542400655469</v>
@@ -9467,10 +9467,10 @@
         <v>1.16340206185567</v>
       </c>
       <c r="AQ42" t="n">
-        <v>1.13609022556391</v>
+        <v>0.8656921451215217</v>
       </c>
       <c r="AR42" t="n">
-        <v>1.13609022556391</v>
+        <v>0.8656921451215217</v>
       </c>
       <c r="AS42" t="n">
         <v>1.386600805678113</v>
@@ -9574,10 +9574,10 @@
         <v>1.128901596378366</v>
       </c>
       <c r="I43" t="n">
-        <v>1.139097744360902</v>
+        <v>0.8629799225079253</v>
       </c>
       <c r="J43" t="n">
-        <v>1.139097744360902</v>
+        <v>0.8629799225079253</v>
       </c>
       <c r="K43" t="n">
         <v>1.396456370340025</v>
@@ -9676,10 +9676,10 @@
         <v>1.165873645255089</v>
       </c>
       <c r="AQ43" t="n">
-        <v>1.139097744360902</v>
+        <v>0.8629799225079253</v>
       </c>
       <c r="AR43" t="n">
-        <v>1.139097744360902</v>
+        <v>0.8629799225079253</v>
       </c>
       <c r="AS43" t="n">
         <v>1.396508728179551</v>
@@ -11194,10 +11194,10 @@
         <v>1.001972308262516</v>
       </c>
       <c r="I6" t="n">
-        <v>1.008354218880535</v>
+        <v>0.9927106571171382</v>
       </c>
       <c r="J6" t="n">
-        <v>1.008354218880535</v>
+        <v>0.9927106571171382</v>
       </c>
       <c r="K6" t="n">
         <v>1.011311393326961</v>
@@ -11296,10 +11296,10 @@
         <v>1.006799424325198</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1.008354218880535</v>
+        <v>0.9927106571171382</v>
       </c>
       <c r="AR6" t="n">
-        <v>1.008354218880535</v>
+        <v>0.9927106571171382</v>
       </c>
       <c r="AS6" t="n">
         <v>1.011315194918686</v>
@@ -11403,10 +11403,10 @@
         <v>1.003944616525031</v>
       </c>
       <c r="I7" t="n">
-        <v>1.016708437761069</v>
+        <v>0.9854213142342766</v>
       </c>
       <c r="J7" t="n">
-        <v>1.016708437761069</v>
+        <v>0.9854213142342766</v>
       </c>
       <c r="K7" t="n">
         <v>1.022622786653921</v>
@@ -11505,10 +11505,10 @@
         <v>1.013598848650395</v>
       </c>
       <c r="AQ7" t="n">
-        <v>1.016708437761069</v>
+        <v>0.9854213142342766</v>
       </c>
       <c r="AR7" t="n">
-        <v>1.016708437761069</v>
+        <v>0.9854213142342766</v>
       </c>
       <c r="AS7" t="n">
         <v>1.022630389837372</v>
@@ -11612,10 +11612,10 @@
         <v>1.005916924787547</v>
       </c>
       <c r="I8" t="n">
-        <v>1.025062656641604</v>
+        <v>0.9781319713514148</v>
       </c>
       <c r="J8" t="n">
-        <v>1.025062656641604</v>
+        <v>0.9781319713514148</v>
       </c>
       <c r="K8" t="n">
         <v>1.033934179980882</v>
@@ -11714,10 +11714,10 @@
         <v>1.020398272975592</v>
       </c>
       <c r="AQ8" t="n">
-        <v>1.025062656641604</v>
+        <v>0.9781319713514148</v>
       </c>
       <c r="AR8" t="n">
-        <v>1.025062656641604</v>
+        <v>0.9781319713514148</v>
       </c>
       <c r="AS8" t="n">
         <v>1.033945584756059</v>
@@ -11821,10 +11821,10 @@
         <v>1.007889233050062</v>
       </c>
       <c r="I9" t="n">
-        <v>1.033416875522139</v>
+        <v>0.9708426284685531</v>
       </c>
       <c r="J9" t="n">
-        <v>1.033416875522139</v>
+        <v>0.9708426284685531</v>
       </c>
       <c r="K9" t="n">
         <v>1.045245573307843</v>
@@ -11923,10 +11923,10 @@
         <v>1.02719769730079</v>
       </c>
       <c r="AQ9" t="n">
-        <v>1.033416875522139</v>
+        <v>0.9708426284685531</v>
       </c>
       <c r="AR9" t="n">
-        <v>1.033416875522139</v>
+        <v>0.9708426284685531</v>
       </c>
       <c r="AS9" t="n">
         <v>1.045260779674745</v>
@@ -12030,10 +12030,10 @@
         <v>1.009861541312578</v>
       </c>
       <c r="I10" t="n">
-        <v>1.041771094402673</v>
+        <v>0.9635532855856913</v>
       </c>
       <c r="J10" t="n">
-        <v>1.041771094402673</v>
+        <v>0.9635532855856913</v>
       </c>
       <c r="K10" t="n">
         <v>1.056556966634804</v>
@@ -12132,10 +12132,10 @@
         <v>1.033997121625988</v>
       </c>
       <c r="AQ10" t="n">
-        <v>1.041771094402673</v>
+        <v>0.9635532855856913</v>
       </c>
       <c r="AR10" t="n">
-        <v>1.041771094402673</v>
+        <v>0.9635532855856913</v>
       </c>
       <c r="AS10" t="n">
         <v>1.056575974593431</v>
@@ -12239,10 +12239,10 @@
         <v>1.011833849575093</v>
       </c>
       <c r="I11" t="n">
-        <v>1.050125313283208</v>
+        <v>0.9562639427028297</v>
       </c>
       <c r="J11" t="n">
-        <v>1.050125313283208</v>
+        <v>0.9562639427028297</v>
       </c>
       <c r="K11" t="n">
         <v>1.067868359961764</v>
@@ -12341,10 +12341,10 @@
         <v>1.040796545951185</v>
       </c>
       <c r="AQ11" t="n">
-        <v>1.050125313283208</v>
+        <v>0.9562639427028297</v>
       </c>
       <c r="AR11" t="n">
-        <v>1.050125313283208</v>
+        <v>0.9562639427028297</v>
       </c>
       <c r="AS11" t="n">
         <v>1.067891169512117</v>
@@ -12448,10 +12448,10 @@
         <v>1.013806157837609</v>
       </c>
       <c r="I12" t="n">
-        <v>1.058479532163743</v>
+        <v>0.9489745998199679</v>
       </c>
       <c r="J12" t="n">
-        <v>1.058479532163743</v>
+        <v>0.9489745998199679</v>
       </c>
       <c r="K12" t="n">
         <v>1.079179753288725</v>
@@ -12550,10 +12550,10 @@
         <v>1.047595970276383</v>
       </c>
       <c r="AQ12" t="n">
-        <v>1.058479532163743</v>
+        <v>0.9489745998199679</v>
       </c>
       <c r="AR12" t="n">
-        <v>1.058479532163743</v>
+        <v>0.9489745998199679</v>
       </c>
       <c r="AS12" t="n">
         <v>1.079206364430803</v>
@@ -12657,10 +12657,10 @@
         <v>1.015778466100124</v>
       </c>
       <c r="I13" t="n">
-        <v>1.066833751044277</v>
+        <v>0.9416852569371061</v>
       </c>
       <c r="J13" t="n">
-        <v>1.066833751044277</v>
+        <v>0.9416852569371061</v>
       </c>
       <c r="K13" t="n">
         <v>1.090491146615686</v>
@@ -12759,10 +12759,10 @@
         <v>1.05439539460158</v>
       </c>
       <c r="AQ13" t="n">
-        <v>1.066833751044277</v>
+        <v>0.9416852569371061</v>
       </c>
       <c r="AR13" t="n">
-        <v>1.066833751044277</v>
+        <v>0.9416852569371061</v>
       </c>
       <c r="AS13" t="n">
         <v>1.090521559349489</v>
@@ -12866,10 +12866,10 @@
         <v>1.01775077436264</v>
       </c>
       <c r="I14" t="n">
-        <v>1.075187969924812</v>
+        <v>0.9343959140542444</v>
       </c>
       <c r="J14" t="n">
-        <v>1.075187969924812</v>
+        <v>0.9343959140542444</v>
       </c>
       <c r="K14" t="n">
         <v>1.101802539942647</v>
@@ -12968,10 +12968,10 @@
         <v>1.061194818926778</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.075187969924812</v>
+        <v>0.9343959140542444</v>
       </c>
       <c r="AR14" t="n">
-        <v>1.075187969924812</v>
+        <v>0.9343959140542444</v>
       </c>
       <c r="AS14" t="n">
         <v>1.101836754268176</v>
@@ -13075,10 +13075,10 @@
         <v>1.019723082625156</v>
       </c>
       <c r="I15" t="n">
-        <v>1.083542188805347</v>
+        <v>0.9271065711713827</v>
       </c>
       <c r="J15" t="n">
-        <v>1.083542188805347</v>
+        <v>0.9271065711713827</v>
       </c>
       <c r="K15" t="n">
         <v>1.113113933269607</v>
@@ -13177,10 +13177,10 @@
         <v>1.067994243251975</v>
       </c>
       <c r="AQ15" t="n">
-        <v>1.083542188805347</v>
+        <v>0.9271065711713827</v>
       </c>
       <c r="AR15" t="n">
-        <v>1.083542188805347</v>
+        <v>0.9271065711713827</v>
       </c>
       <c r="AS15" t="n">
         <v>1.113151949186862</v>
@@ -13284,10 +13284,10 @@
         <v>1.021695390887671</v>
       </c>
       <c r="I16" t="n">
-        <v>1.091896407685881</v>
+        <v>0.919817228288521</v>
       </c>
       <c r="J16" t="n">
-        <v>1.091896407685881</v>
+        <v>0.919817228288521</v>
       </c>
       <c r="K16" t="n">
         <v>1.124425326596568</v>
@@ -13386,10 +13386,10 @@
         <v>1.074793667577173</v>
       </c>
       <c r="AQ16" t="n">
-        <v>1.091896407685881</v>
+        <v>0.919817228288521</v>
       </c>
       <c r="AR16" t="n">
-        <v>1.091896407685881</v>
+        <v>0.919817228288521</v>
       </c>
       <c r="AS16" t="n">
         <v>1.124467144105548</v>
@@ -13493,10 +13493,10 @@
         <v>1.023667699150187</v>
       </c>
       <c r="I17" t="n">
-        <v>1.100250626566416</v>
+        <v>0.9125278854056592</v>
       </c>
       <c r="J17" t="n">
-        <v>1.100250626566416</v>
+        <v>0.9125278854056592</v>
       </c>
       <c r="K17" t="n">
         <v>1.135736719923529</v>
@@ -13595,10 +13595,10 @@
         <v>1.08159309190237</v>
       </c>
       <c r="AQ17" t="n">
-        <v>1.100250626566416</v>
+        <v>0.9125278854056592</v>
       </c>
       <c r="AR17" t="n">
-        <v>1.100250626566416</v>
+        <v>0.9125278854056592</v>
       </c>
       <c r="AS17" t="n">
         <v>1.135782339024234</v>
@@ -13702,10 +13702,10 @@
         <v>1.025640007412702</v>
       </c>
       <c r="I18" t="n">
-        <v>1.108604845446951</v>
+        <v>0.9052385425227976</v>
       </c>
       <c r="J18" t="n">
-        <v>1.108604845446951</v>
+        <v>0.9052385425227976</v>
       </c>
       <c r="K18" t="n">
         <v>1.147048113250489</v>
@@ -13804,10 +13804,10 @@
         <v>1.088392516227568</v>
       </c>
       <c r="AQ18" t="n">
-        <v>1.108604845446951</v>
+        <v>0.9052385425227976</v>
       </c>
       <c r="AR18" t="n">
-        <v>1.108604845446951</v>
+        <v>0.9052385425227976</v>
       </c>
       <c r="AS18" t="n">
         <v>1.147097533942921</v>
@@ -13911,10 +13911,10 @@
         <v>1.027612315675218</v>
       </c>
       <c r="I19" t="n">
-        <v>1.116959064327485</v>
+        <v>0.8979491996399358</v>
       </c>
       <c r="J19" t="n">
-        <v>1.116959064327485</v>
+        <v>0.8979491996399358</v>
       </c>
       <c r="K19" t="n">
         <v>1.15835950657745</v>
@@ -14013,10 +14013,10 @@
         <v>1.095191940552765</v>
       </c>
       <c r="AQ19" t="n">
-        <v>1.116959064327485</v>
+        <v>0.8979491996399358</v>
       </c>
       <c r="AR19" t="n">
-        <v>1.116959064327485</v>
+        <v>0.8979491996399358</v>
       </c>
       <c r="AS19" t="n">
         <v>1.158412728861607</v>
@@ -14120,10 +14120,10 @@
         <v>1.029584623937733</v>
       </c>
       <c r="I20" t="n">
-        <v>1.12531328320802</v>
+        <v>0.890659856757074</v>
       </c>
       <c r="J20" t="n">
-        <v>1.12531328320802</v>
+        <v>0.890659856757074</v>
       </c>
       <c r="K20" t="n">
         <v>1.169670899904411</v>
@@ -14222,10 +14222,10 @@
         <v>1.101991364877963</v>
       </c>
       <c r="AQ20" t="n">
-        <v>1.12531328320802</v>
+        <v>0.890659856757074</v>
       </c>
       <c r="AR20" t="n">
-        <v>1.12531328320802</v>
+        <v>0.890659856757074</v>
       </c>
       <c r="AS20" t="n">
         <v>1.169727923780293</v>
@@ -14329,10 +14329,10 @@
         <v>1.031556932200249</v>
       </c>
       <c r="I21" t="n">
-        <v>1.133667502088555</v>
+        <v>0.8833705138742123</v>
       </c>
       <c r="J21" t="n">
-        <v>1.133667502088555</v>
+        <v>0.8833705138742123</v>
       </c>
       <c r="K21" t="n">
         <v>1.180982293231372</v>
@@ -14431,10 +14431,10 @@
         <v>1.108790789203161</v>
       </c>
       <c r="AQ21" t="n">
-        <v>1.133667502088555</v>
+        <v>0.8833705138742123</v>
       </c>
       <c r="AR21" t="n">
-        <v>1.133667502088555</v>
+        <v>0.8833705138742123</v>
       </c>
       <c r="AS21" t="n">
         <v>1.181043118698979</v>
@@ -14538,10 +14538,10 @@
         <v>1.033529240462764</v>
       </c>
       <c r="I22" t="n">
-        <v>1.142021720969089</v>
+        <v>0.8760811709913506</v>
       </c>
       <c r="J22" t="n">
-        <v>1.142021720969089</v>
+        <v>0.8760811709913506</v>
       </c>
       <c r="K22" t="n">
         <v>1.192293686558332</v>
@@ -14640,10 +14640,10 @@
         <v>1.115590213528358</v>
       </c>
       <c r="AQ22" t="n">
-        <v>1.142021720969089</v>
+        <v>0.8760811709913506</v>
       </c>
       <c r="AR22" t="n">
-        <v>1.142021720969089</v>
+        <v>0.8760811709913506</v>
       </c>
       <c r="AS22" t="n">
         <v>1.192358313617665</v>
@@ -14747,10 +14747,10 @@
         <v>1.03550154872528</v>
       </c>
       <c r="I23" t="n">
-        <v>1.150375939849624</v>
+        <v>0.8687918281084889</v>
       </c>
       <c r="J23" t="n">
-        <v>1.150375939849624</v>
+        <v>0.8687918281084889</v>
       </c>
       <c r="K23" t="n">
         <v>1.203605079885293</v>
@@ -14849,10 +14849,10 @@
         <v>1.122389637853556</v>
       </c>
       <c r="AQ23" t="n">
-        <v>1.150375939849624</v>
+        <v>0.8687918281084889</v>
       </c>
       <c r="AR23" t="n">
-        <v>1.150375939849624</v>
+        <v>0.8687918281084889</v>
       </c>
       <c r="AS23" t="n">
         <v>1.203673508536351</v>
@@ -14956,10 +14956,10 @@
         <v>1.034786752442221</v>
       </c>
       <c r="I24" t="n">
-        <v>1.152631578947368</v>
+        <v>0.8658330398027474</v>
       </c>
       <c r="J24" t="n">
-        <v>1.152631578947368</v>
+        <v>0.8658330398027474</v>
       </c>
       <c r="K24" t="n">
         <v>1.214748054076198</v>
@@ -15058,10 +15058,10 @@
         <v>1.126883425852498</v>
       </c>
       <c r="AQ24" t="n">
-        <v>1.152631578947368</v>
+        <v>0.8658330398027474</v>
       </c>
       <c r="AR24" t="n">
-        <v>1.152631578947368</v>
+        <v>0.8658330398027474</v>
       </c>
       <c r="AS24" t="n">
         <v>1.214828313830808</v>
@@ -15165,10 +15165,10 @@
         <v>1.034071956159161</v>
       </c>
       <c r="I25" t="n">
-        <v>1.154887218045113</v>
+        <v>0.8628742514970059</v>
       </c>
       <c r="J25" t="n">
-        <v>1.154887218045113</v>
+        <v>0.8628742514970059</v>
       </c>
       <c r="K25" t="n">
         <v>1.225891028267104</v>
@@ -15267,10 +15267,10 @@
         <v>1.131377213851441</v>
       </c>
       <c r="AQ25" t="n">
-        <v>1.154887218045113</v>
+        <v>0.8628742514970059</v>
       </c>
       <c r="AR25" t="n">
-        <v>1.154887218045113</v>
+        <v>0.8628742514970059</v>
       </c>
       <c r="AS25" t="n">
         <v>1.225983119125264</v>
@@ -15374,10 +15374,10 @@
         <v>1.033357159876102</v>
       </c>
       <c r="I26" t="n">
-        <v>1.157142857142857</v>
+        <v>0.8599154631912646</v>
       </c>
       <c r="J26" t="n">
-        <v>1.157142857142857</v>
+        <v>0.8599154631912646</v>
       </c>
       <c r="K26" t="n">
         <v>1.237034002458009</v>
@@ -15476,10 +15476,10 @@
         <v>1.135871001850383</v>
       </c>
       <c r="AQ26" t="n">
-        <v>1.157142857142857</v>
+        <v>0.8599154631912646</v>
       </c>
       <c r="AR26" t="n">
-        <v>1.157142857142857</v>
+        <v>0.8599154631912646</v>
       </c>
       <c r="AS26" t="n">
         <v>1.23713792441972</v>
@@ -15583,10 +15583,10 @@
         <v>1.032642363593043</v>
       </c>
       <c r="I27" t="n">
-        <v>1.159398496240601</v>
+        <v>0.8569566748855231</v>
       </c>
       <c r="J27" t="n">
-        <v>1.159398496240601</v>
+        <v>0.8569566748855231</v>
       </c>
       <c r="K27" t="n">
         <v>1.248176976648915</v>
@@ -15685,10 +15685,10 @@
         <v>1.140364789849326</v>
       </c>
       <c r="AQ27" t="n">
-        <v>1.159398496240601</v>
+        <v>0.8569566748855231</v>
       </c>
       <c r="AR27" t="n">
-        <v>1.159398496240601</v>
+        <v>0.8569566748855231</v>
       </c>
       <c r="AS27" t="n">
         <v>1.248292729714176</v>
@@ -15792,10 +15792,10 @@
         <v>1.031927567309983</v>
       </c>
       <c r="I28" t="n">
-        <v>1.161654135338346</v>
+        <v>0.8539978865797816</v>
       </c>
       <c r="J28" t="n">
-        <v>1.161654135338346</v>
+        <v>0.8539978865797816</v>
       </c>
       <c r="K28" t="n">
         <v>1.25931995083982</v>
@@ -15894,10 +15894,10 @@
         <v>1.144858577848269</v>
       </c>
       <c r="AQ28" t="n">
-        <v>1.161654135338346</v>
+        <v>0.8539978865797816</v>
       </c>
       <c r="AR28" t="n">
-        <v>1.161654135338346</v>
+        <v>0.8539978865797816</v>
       </c>
       <c r="AS28" t="n">
         <v>1.259447535008632</v>
@@ -16001,10 +16001,10 @@
         <v>1.030545627829402</v>
       </c>
       <c r="I29" t="n">
-        <v>1.16390977443609</v>
+        <v>0.8535047551954914</v>
       </c>
       <c r="J29" t="n">
-        <v>1.16390977443609</v>
+        <v>0.8535047551954914</v>
       </c>
       <c r="K29" t="n">
         <v>1.270503891847603</v>
@@ -16103,10 +16103,10 @@
         <v>1.148717948717949</v>
       </c>
       <c r="AQ29" t="n">
-        <v>1.16390977443609</v>
+        <v>0.8535047551954914</v>
       </c>
       <c r="AR29" t="n">
-        <v>1.16390977443609</v>
+        <v>0.8535047551954914</v>
       </c>
       <c r="AS29" t="n">
         <v>1.270631114521389</v>
@@ -16210,10 +16210,10 @@
         <v>1.029163688348821</v>
       </c>
       <c r="I30" t="n">
-        <v>1.166165413533835</v>
+        <v>0.8530116238112011</v>
       </c>
       <c r="J30" t="n">
-        <v>1.166165413533835</v>
+        <v>0.8530116238112011</v>
       </c>
       <c r="K30" t="n">
         <v>1.281687832855387</v>
@@ -16312,10 +16312,10 @@
         <v>1.152577319587629</v>
       </c>
       <c r="AQ30" t="n">
-        <v>1.166165413533835</v>
+        <v>0.8530116238112011</v>
       </c>
       <c r="AR30" t="n">
-        <v>1.166165413533835</v>
+        <v>0.8530116238112011</v>
       </c>
       <c r="AS30" t="n">
         <v>1.281814694034145</v>
@@ -16419,10 +16419,10 @@
         <v>1.027781748868239</v>
       </c>
       <c r="I31" t="n">
-        <v>1.168421052631579</v>
+        <v>0.8525184924269109</v>
       </c>
       <c r="J31" t="n">
-        <v>1.168421052631579</v>
+        <v>0.8525184924269109</v>
       </c>
       <c r="K31" t="n">
         <v>1.292871773863171</v>
@@ -16521,10 +16521,10 @@
         <v>1.156436690457309</v>
       </c>
       <c r="AQ31" t="n">
-        <v>1.168421052631579</v>
+        <v>0.8525184924269109</v>
       </c>
       <c r="AR31" t="n">
-        <v>1.168421052631579</v>
+        <v>0.8525184924269109</v>
       </c>
       <c r="AS31" t="n">
         <v>1.292998273546902</v>
@@ -16628,10 +16628,10 @@
         <v>1.026399809387658</v>
       </c>
       <c r="I32" t="n">
-        <v>1.170676691729323</v>
+        <v>0.8520253610426206</v>
       </c>
       <c r="J32" t="n">
-        <v>1.170676691729323</v>
+        <v>0.8520253610426206</v>
       </c>
       <c r="K32" t="n">
         <v>1.304055714870955</v>
@@ -16730,10 +16730,10 @@
         <v>1.160296061326989</v>
       </c>
       <c r="AQ32" t="n">
-        <v>1.170676691729323</v>
+        <v>0.8520253610426206</v>
       </c>
       <c r="AR32" t="n">
-        <v>1.170676691729323</v>
+        <v>0.8520253610426206</v>
       </c>
       <c r="AS32" t="n">
         <v>1.304181853059659</v>
@@ -16837,10 +16837,10 @@
         <v>1.025017869907076</v>
       </c>
       <c r="I33" t="n">
-        <v>1.172932330827068</v>
+        <v>0.8515322296583304</v>
       </c>
       <c r="J33" t="n">
-        <v>1.172932330827068</v>
+        <v>0.8515322296583304</v>
       </c>
       <c r="K33" t="n">
         <v>1.315239655878738</v>
@@ -16939,10 +16939,10 @@
         <v>1.164155432196669</v>
       </c>
       <c r="AQ33" t="n">
-        <v>1.172932330827068</v>
+        <v>0.8515322296583304</v>
       </c>
       <c r="AR33" t="n">
-        <v>1.172932330827068</v>
+        <v>0.8515322296583304</v>
       </c>
       <c r="AS33" t="n">
         <v>1.315365432572415</v>
@@ -17046,10 +17046,10 @@
         <v>1.022825827972361</v>
       </c>
       <c r="I34" t="n">
-        <v>1.175187969924812</v>
+        <v>0.8526065516026771</v>
       </c>
       <c r="J34" t="n">
-        <v>1.175187969924812</v>
+        <v>0.8526065516026771</v>
       </c>
       <c r="K34" t="n">
         <v>1.326034412126178</v>
@@ -17148,10 +17148,10 @@
         <v>1.167287866772403</v>
       </c>
       <c r="AQ34" t="n">
-        <v>1.175187969924812</v>
+        <v>0.8526065516026771</v>
       </c>
       <c r="AR34" t="n">
-        <v>1.175187969924812</v>
+        <v>0.8526065516026771</v>
       </c>
       <c r="AS34" t="n">
         <v>1.326155764435066</v>
@@ -17255,10 +17255,10 @@
         <v>1.020633786037646</v>
       </c>
       <c r="I35" t="n">
-        <v>1.177443609022556</v>
+        <v>0.8536808735470236</v>
       </c>
       <c r="J35" t="n">
-        <v>1.177443609022556</v>
+        <v>0.8536808735470236</v>
       </c>
       <c r="K35" t="n">
         <v>1.336829168373618</v>
@@ -17357,10 +17357,10 @@
         <v>1.170420301348136</v>
       </c>
       <c r="AQ35" t="n">
-        <v>1.177443609022556</v>
+        <v>0.8536808735470236</v>
       </c>
       <c r="AR35" t="n">
-        <v>1.177443609022556</v>
+        <v>0.8536808735470236</v>
       </c>
       <c r="AS35" t="n">
         <v>1.336946096297717</v>
@@ -17464,10 +17464,10 @@
         <v>1.018441744102931</v>
       </c>
       <c r="I36" t="n">
-        <v>1.179699248120301</v>
+        <v>0.8547551954913702</v>
       </c>
       <c r="J36" t="n">
-        <v>1.179699248120301</v>
+        <v>0.8547551954913702</v>
       </c>
       <c r="K36" t="n">
         <v>1.347623924621057</v>
@@ -17566,10 +17566,10 @@
         <v>1.17355273592387</v>
       </c>
       <c r="AQ36" t="n">
-        <v>1.179699248120301</v>
+        <v>0.8547551954913702</v>
       </c>
       <c r="AR36" t="n">
-        <v>1.179699248120301</v>
+        <v>0.8547551954913702</v>
       </c>
       <c r="AS36" t="n">
         <v>1.347736428160368</v>
@@ -17673,10 +17673,10 @@
         <v>1.016249702168215</v>
       </c>
       <c r="I37" t="n">
-        <v>1.181954887218045</v>
+        <v>0.8558295174357168</v>
       </c>
       <c r="J37" t="n">
-        <v>1.181954887218045</v>
+        <v>0.8558295174357168</v>
       </c>
       <c r="K37" t="n">
         <v>1.358418680868497</v>
@@ -17775,10 +17775,10 @@
         <v>1.176685170499604</v>
       </c>
       <c r="AQ37" t="n">
-        <v>1.181954887218045</v>
+        <v>0.8558295174357168</v>
       </c>
       <c r="AR37" t="n">
-        <v>1.181954887218045</v>
+        <v>0.8558295174357168</v>
       </c>
       <c r="AS37" t="n">
         <v>1.358526760023019</v>
@@ -17882,10 +17882,10 @@
         <v>1.0140576602335</v>
       </c>
       <c r="I38" t="n">
-        <v>1.184210526315789</v>
+        <v>0.8569038393800634</v>
       </c>
       <c r="J38" t="n">
-        <v>1.184210526315789</v>
+        <v>0.8569038393800634</v>
       </c>
       <c r="K38" t="n">
         <v>1.369213437115936</v>
@@ -17984,10 +17984,10 @@
         <v>1.179817605075337</v>
       </c>
       <c r="AQ38" t="n">
-        <v>1.184210526315789</v>
+        <v>0.8569038393800634</v>
       </c>
       <c r="AR38" t="n">
-        <v>1.184210526315789</v>
+        <v>0.8569038393800634</v>
       </c>
       <c r="AS38" t="n">
         <v>1.36931709188567</v>
@@ -18091,10 +18091,10 @@
         <v>1.011865618298785</v>
       </c>
       <c r="I39" t="n">
-        <v>1.186466165413534</v>
+        <v>0.8579781613244101</v>
       </c>
       <c r="J39" t="n">
-        <v>1.186466165413534</v>
+        <v>0.8579781613244101</v>
       </c>
       <c r="K39" t="n">
         <v>1.380008193363376</v>
@@ -18193,10 +18193,10 @@
         <v>1.182950039651071</v>
       </c>
       <c r="AQ39" t="n">
-        <v>1.186466165413534</v>
+        <v>0.8579781613244101</v>
       </c>
       <c r="AR39" t="n">
-        <v>1.186466165413534</v>
+        <v>0.8579781613244101</v>
       </c>
       <c r="AS39" t="n">
         <v>1.380107423748322</v>
@@ -18300,10 +18300,10 @@
         <v>1.00967357636407</v>
       </c>
       <c r="I40" t="n">
-        <v>1.188721804511278</v>
+        <v>0.8590524832687566</v>
       </c>
       <c r="J40" t="n">
-        <v>1.188721804511278</v>
+        <v>0.8590524832687566</v>
       </c>
       <c r="K40" t="n">
         <v>1.390802949610815</v>
@@ -18402,10 +18402,10 @@
         <v>1.186082474226804</v>
       </c>
       <c r="AQ40" t="n">
-        <v>1.188721804511278</v>
+        <v>0.8590524832687566</v>
       </c>
       <c r="AR40" t="n">
-        <v>1.188721804511278</v>
+        <v>0.8590524832687566</v>
       </c>
       <c r="AS40" t="n">
         <v>1.390897755610973</v>
@@ -18509,10 +18509,10 @@
         <v>1.007481534429354</v>
       </c>
       <c r="I41" t="n">
-        <v>1.190977443609023</v>
+        <v>0.8601268052131033</v>
       </c>
       <c r="J41" t="n">
-        <v>1.190977443609023</v>
+        <v>0.8601268052131033</v>
       </c>
       <c r="K41" t="n">
         <v>1.401597705858255</v>
@@ -18611,10 +18611,10 @@
         <v>1.189214908802538</v>
       </c>
       <c r="AQ41" t="n">
-        <v>1.190977443609023</v>
+        <v>0.8601268052131033</v>
       </c>
       <c r="AR41" t="n">
-        <v>1.190977443609023</v>
+        <v>0.8601268052131033</v>
       </c>
       <c r="AS41" t="n">
         <v>1.401688087473624</v>
@@ -18718,10 +18718,10 @@
         <v>1.005289492494639</v>
       </c>
       <c r="I42" t="n">
-        <v>1.193233082706767</v>
+        <v>0.8612011271574498</v>
       </c>
       <c r="J42" t="n">
-        <v>1.193233082706767</v>
+        <v>0.8612011271574498</v>
       </c>
       <c r="K42" t="n">
         <v>1.412392462105695</v>
@@ -18820,10 +18820,10 @@
         <v>1.192347343378271</v>
       </c>
       <c r="AQ42" t="n">
-        <v>1.193233082706767</v>
+        <v>0.8612011271574498</v>
       </c>
       <c r="AR42" t="n">
-        <v>1.193233082706767</v>
+        <v>0.8612011271574498</v>
       </c>
       <c r="AS42" t="n">
         <v>1.412478419336275</v>
@@ -18927,10 +18927,10 @@
         <v>1.003097450559924</v>
       </c>
       <c r="I43" t="n">
-        <v>1.195488721804511</v>
+        <v>0.8622754491017964</v>
       </c>
       <c r="J43" t="n">
-        <v>1.195488721804511</v>
+        <v>0.8622754491017964</v>
       </c>
       <c r="K43" t="n">
         <v>1.423187218353134</v>
@@ -19029,10 +19029,10 @@
         <v>1.195479777954005</v>
       </c>
       <c r="AQ43" t="n">
-        <v>1.195488721804511</v>
+        <v>0.8622754491017964</v>
       </c>
       <c r="AR43" t="n">
-        <v>1.195488721804511</v>
+        <v>0.8622754491017964</v>
       </c>
       <c r="AS43" t="n">
         <v>1.423268751198926</v>
@@ -20547,10 +20547,10 @@
         <v>0.9956979853334392</v>
       </c>
       <c r="I6" t="n">
-        <v>1.00125313283208</v>
+        <v>0.9974756369613714</v>
       </c>
       <c r="J6" t="n">
-        <v>1.00125313283208</v>
+        <v>0.9974756369613714</v>
       </c>
       <c r="K6" t="n">
         <v>0.9989189312212663</v>
@@ -20649,10 +20649,10 @@
         <v>0.9946324198901518</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1.00125313283208</v>
+        <v>0.9974756369613714</v>
       </c>
       <c r="AR6" t="n">
-        <v>1.00125313283208</v>
+        <v>0.9974756369613714</v>
       </c>
       <c r="AS6" t="n">
         <v>0.9989236310932071</v>
@@ -20756,10 +20756,10 @@
         <v>0.9913959706668785</v>
       </c>
       <c r="I7" t="n">
-        <v>1.00250626566416</v>
+        <v>0.9949512739227427</v>
       </c>
       <c r="J7" t="n">
-        <v>1.00250626566416</v>
+        <v>0.9949512739227427</v>
       </c>
       <c r="K7" t="n">
         <v>0.9978378624425327</v>
@@ -20858,10 +20858,10 @@
         <v>0.9892648397803037</v>
       </c>
       <c r="AQ7" t="n">
-        <v>1.00250626566416</v>
+        <v>0.9949512739227427</v>
       </c>
       <c r="AR7" t="n">
-        <v>1.00250626566416</v>
+        <v>0.9949512739227427</v>
       </c>
       <c r="AS7" t="n">
         <v>0.9978472621864143</v>
@@ -20965,10 +20965,10 @@
         <v>0.9870939560003177</v>
       </c>
       <c r="I8" t="n">
-        <v>1.003759398496241</v>
+        <v>0.9924269108841142</v>
       </c>
       <c r="J8" t="n">
-        <v>1.003759398496241</v>
+        <v>0.9924269108841142</v>
       </c>
       <c r="K8" t="n">
         <v>0.996756793663799</v>
@@ -21067,10 +21067,10 @@
         <v>0.9838972596704556</v>
       </c>
       <c r="AQ8" t="n">
-        <v>1.003759398496241</v>
+        <v>0.9924269108841142</v>
       </c>
       <c r="AR8" t="n">
-        <v>1.003759398496241</v>
+        <v>0.9924269108841142</v>
       </c>
       <c r="AS8" t="n">
         <v>0.9967708932796214</v>
@@ -21174,10 +21174,10 @@
         <v>0.9827919413337569</v>
       </c>
       <c r="I9" t="n">
-        <v>1.005012531328321</v>
+        <v>0.9899025478454855</v>
       </c>
       <c r="J9" t="n">
-        <v>1.005012531328321</v>
+        <v>0.9899025478454855</v>
       </c>
       <c r="K9" t="n">
         <v>0.9956757248850653</v>
@@ -21276,10 +21276,10 @@
         <v>0.9785296795606074</v>
       </c>
       <c r="AQ9" t="n">
-        <v>1.005012531328321</v>
+        <v>0.9899025478454855</v>
       </c>
       <c r="AR9" t="n">
-        <v>1.005012531328321</v>
+        <v>0.9899025478454855</v>
       </c>
       <c r="AS9" t="n">
         <v>0.9956945243728286</v>
@@ -21383,10 +21383,10 @@
         <v>0.9784899266671961</v>
       </c>
       <c r="I10" t="n">
-        <v>1.006265664160401</v>
+        <v>0.9873781848068569</v>
       </c>
       <c r="J10" t="n">
-        <v>1.006265664160401</v>
+        <v>0.9873781848068569</v>
       </c>
       <c r="K10" t="n">
         <v>0.9945946561063317</v>
@@ -21485,10 +21485,10 @@
         <v>0.9731620994507593</v>
       </c>
       <c r="AQ10" t="n">
-        <v>1.006265664160401</v>
+        <v>0.9873781848068569</v>
       </c>
       <c r="AR10" t="n">
-        <v>1.006265664160401</v>
+        <v>0.9873781848068569</v>
       </c>
       <c r="AS10" t="n">
         <v>0.9946181554660358</v>
@@ -21592,10 +21592,10 @@
         <v>0.9741879120006354</v>
       </c>
       <c r="I11" t="n">
-        <v>1.007518796992481</v>
+        <v>0.9848538217682282</v>
       </c>
       <c r="J11" t="n">
-        <v>1.007518796992481</v>
+        <v>0.9848538217682282</v>
       </c>
       <c r="K11" t="n">
         <v>0.993513587327598</v>
@@ -21694,10 +21694,10 @@
         <v>0.9677945193409111</v>
       </c>
       <c r="AQ11" t="n">
-        <v>1.007518796992481</v>
+        <v>0.9848538217682282</v>
       </c>
       <c r="AR11" t="n">
-        <v>1.007518796992481</v>
+        <v>0.9848538217682282</v>
       </c>
       <c r="AS11" t="n">
         <v>0.993541786559243</v>
@@ -21801,10 +21801,10 @@
         <v>0.9698858973340746</v>
       </c>
       <c r="I12" t="n">
-        <v>1.008771929824561</v>
+        <v>0.9823294587295996</v>
       </c>
       <c r="J12" t="n">
-        <v>1.008771929824561</v>
+        <v>0.9823294587295996</v>
       </c>
       <c r="K12" t="n">
         <v>0.9924325185488643</v>
@@ -21903,10 +21903,10 @@
         <v>0.9624269392310629</v>
       </c>
       <c r="AQ12" t="n">
-        <v>1.008771929824561</v>
+        <v>0.9823294587295996</v>
       </c>
       <c r="AR12" t="n">
-        <v>1.008771929824561</v>
+        <v>0.9823294587295996</v>
       </c>
       <c r="AS12" t="n">
         <v>0.9924654176524501</v>
@@ -22010,10 +22010,10 @@
         <v>0.9655838826675138</v>
       </c>
       <c r="I13" t="n">
-        <v>1.010025062656642</v>
+        <v>0.979805095690971</v>
       </c>
       <c r="J13" t="n">
-        <v>1.010025062656642</v>
+        <v>0.979805095690971</v>
       </c>
       <c r="K13" t="n">
         <v>0.9913514497701307</v>
@@ -22112,10 +22112,10 @@
         <v>0.9570593591212148</v>
       </c>
       <c r="AQ13" t="n">
-        <v>1.010025062656642</v>
+        <v>0.979805095690971</v>
       </c>
       <c r="AR13" t="n">
-        <v>1.010025062656642</v>
+        <v>0.979805095690971</v>
       </c>
       <c r="AS13" t="n">
         <v>0.9913890487456573</v>
@@ -22219,10 +22219,10 @@
         <v>0.9612818680009531</v>
       </c>
       <c r="I14" t="n">
-        <v>1.011278195488722</v>
+        <v>0.9772807326523424</v>
       </c>
       <c r="J14" t="n">
-        <v>1.011278195488722</v>
+        <v>0.9772807326523424</v>
       </c>
       <c r="K14" t="n">
         <v>0.990270380991397</v>
@@ -22321,10 +22321,10 @@
         <v>0.9516917790113666</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.011278195488722</v>
+        <v>0.9772807326523424</v>
       </c>
       <c r="AR14" t="n">
-        <v>1.011278195488722</v>
+        <v>0.9772807326523424</v>
       </c>
       <c r="AS14" t="n">
         <v>0.9903126798388644</v>
@@ -22428,10 +22428,10 @@
         <v>0.9569798533343923</v>
       </c>
       <c r="I15" t="n">
-        <v>1.012531328320802</v>
+        <v>0.9747563696137138</v>
       </c>
       <c r="J15" t="n">
-        <v>1.012531328320802</v>
+        <v>0.9747563696137138</v>
       </c>
       <c r="K15" t="n">
         <v>0.9891893122126633</v>
@@ -22530,10 +22530,10 @@
         <v>0.9463241989015185</v>
       </c>
       <c r="AQ15" t="n">
-        <v>1.012531328320802</v>
+        <v>0.9747563696137138</v>
       </c>
       <c r="AR15" t="n">
-        <v>1.012531328320802</v>
+        <v>0.9747563696137138</v>
       </c>
       <c r="AS15" t="n">
         <v>0.9892363109320715</v>
@@ -22637,10 +22637,10 @@
         <v>0.9526778386678315</v>
       </c>
       <c r="I16" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9722320065750851</v>
       </c>
       <c r="J16" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9722320065750851</v>
       </c>
       <c r="K16" t="n">
         <v>0.9881082434339297</v>
@@ -22739,10 +22739,10 @@
         <v>0.9409566187916704</v>
       </c>
       <c r="AQ16" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9722320065750851</v>
       </c>
       <c r="AR16" t="n">
-        <v>1.013784461152882</v>
+        <v>0.9722320065750851</v>
       </c>
       <c r="AS16" t="n">
         <v>0.9881599420252787</v>
@@ -22846,10 +22846,10 @@
         <v>0.9483758240012707</v>
       </c>
       <c r="I17" t="n">
-        <v>1.015037593984962</v>
+        <v>0.9697076435364566</v>
       </c>
       <c r="J17" t="n">
-        <v>1.015037593984962</v>
+        <v>0.9697076435364566</v>
       </c>
       <c r="K17" t="n">
         <v>0.987027174655196</v>
@@ -22948,10 +22948,10 @@
         <v>0.9355890386818222</v>
       </c>
       <c r="AQ17" t="n">
-        <v>1.015037593984962</v>
+        <v>0.9697076435364566</v>
       </c>
       <c r="AR17" t="n">
-        <v>1.015037593984962</v>
+        <v>0.9697076435364566</v>
       </c>
       <c r="AS17" t="n">
         <v>0.9870835731184858</v>
@@ -23055,10 +23055,10 @@
         <v>0.94407380933471</v>
       </c>
       <c r="I18" t="n">
-        <v>1.016290726817042</v>
+        <v>0.9671832804978279</v>
       </c>
       <c r="J18" t="n">
-        <v>1.016290726817042</v>
+        <v>0.9671832804978279</v>
       </c>
       <c r="K18" t="n">
         <v>0.9859461058764623</v>
@@ -23157,10 +23157,10 @@
         <v>0.930221458571974</v>
       </c>
       <c r="AQ18" t="n">
-        <v>1.016290726817042</v>
+        <v>0.9671832804978279</v>
       </c>
       <c r="AR18" t="n">
-        <v>1.016290726817042</v>
+        <v>0.9671832804978279</v>
       </c>
       <c r="AS18" t="n">
         <v>0.986007204211693</v>
@@ -23264,10 +23264,10 @@
         <v>0.9397717946681492</v>
       </c>
       <c r="I19" t="n">
-        <v>1.017543859649123</v>
+        <v>0.9646589174591993</v>
       </c>
       <c r="J19" t="n">
-        <v>1.017543859649123</v>
+        <v>0.9646589174591993</v>
       </c>
       <c r="K19" t="n">
         <v>0.9848650370977287</v>
@@ -23366,10 +23366,10 @@
         <v>0.9248538784621259</v>
       </c>
       <c r="AQ19" t="n">
-        <v>1.017543859649123</v>
+        <v>0.9646589174591993</v>
       </c>
       <c r="AR19" t="n">
-        <v>1.017543859649123</v>
+        <v>0.9646589174591993</v>
       </c>
       <c r="AS19" t="n">
         <v>0.9849308353049002</v>
@@ -23473,10 +23473,10 @@
         <v>0.9354697800015884</v>
       </c>
       <c r="I20" t="n">
-        <v>1.018796992481203</v>
+        <v>0.9621345544205706</v>
       </c>
       <c r="J20" t="n">
-        <v>1.018796992481203</v>
+        <v>0.9621345544205706</v>
       </c>
       <c r="K20" t="n">
         <v>0.983783968318995</v>
@@ -23575,10 +23575,10 @@
         <v>0.9194862983522778</v>
       </c>
       <c r="AQ20" t="n">
-        <v>1.018796992481203</v>
+        <v>0.9621345544205706</v>
       </c>
       <c r="AR20" t="n">
-        <v>1.018796992481203</v>
+        <v>0.9621345544205706</v>
       </c>
       <c r="AS20" t="n">
         <v>0.9838544663981074</v>
@@ -23682,10 +23682,10 @@
         <v>0.9311677653350277</v>
       </c>
       <c r="I21" t="n">
-        <v>1.020050125313283</v>
+        <v>0.959610191381942</v>
       </c>
       <c r="J21" t="n">
-        <v>1.020050125313283</v>
+        <v>0.959610191381942</v>
       </c>
       <c r="K21" t="n">
         <v>0.9827028995402612</v>
@@ -23784,10 +23784,10 @@
         <v>0.9141187182424296</v>
       </c>
       <c r="AQ21" t="n">
-        <v>1.020050125313283</v>
+        <v>0.959610191381942</v>
       </c>
       <c r="AR21" t="n">
-        <v>1.020050125313283</v>
+        <v>0.959610191381942</v>
       </c>
       <c r="AS21" t="n">
         <v>0.9827780974913145</v>
@@ -23891,10 +23891,10 @@
         <v>0.9268657506684669</v>
       </c>
       <c r="I22" t="n">
-        <v>1.021303258145363</v>
+        <v>0.9570858283433133</v>
       </c>
       <c r="J22" t="n">
-        <v>1.021303258145363</v>
+        <v>0.9570858283433133</v>
       </c>
       <c r="K22" t="n">
         <v>0.9816218307615276</v>
@@ -23993,10 +23993,10 @@
         <v>0.9087511381325815</v>
       </c>
       <c r="AQ22" t="n">
-        <v>1.021303258145363</v>
+        <v>0.9570858283433133</v>
       </c>
       <c r="AR22" t="n">
-        <v>1.021303258145363</v>
+        <v>0.9570858283433133</v>
       </c>
       <c r="AS22" t="n">
         <v>0.9817017285845216</v>
@@ -24100,10 +24100,10 @@
         <v>0.9225637360019061</v>
       </c>
       <c r="I23" t="n">
-        <v>1.022556390977444</v>
+        <v>0.9545614653046848</v>
       </c>
       <c r="J23" t="n">
-        <v>1.022556390977444</v>
+        <v>0.9545614653046848</v>
       </c>
       <c r="K23" t="n">
         <v>0.9805407619827939</v>
@@ -24202,10 +24202,10 @@
         <v>0.9033835580227333</v>
       </c>
       <c r="AQ23" t="n">
-        <v>1.022556390977444</v>
+        <v>0.9545614653046848</v>
       </c>
       <c r="AR23" t="n">
-        <v>1.022556390977444</v>
+        <v>0.9545614653046848</v>
       </c>
       <c r="AS23" t="n">
         <v>0.9806253596777288</v>
@@ -24309,10 +24309,10 @@
         <v>0.9241362878246366</v>
       </c>
       <c r="I24" t="n">
-        <v>1.021052631578947</v>
+        <v>0.9433955618175414</v>
       </c>
       <c r="J24" t="n">
-        <v>1.021052631578947</v>
+        <v>0.9433955618175414</v>
       </c>
       <c r="K24" t="n">
         <v>0.9864399836132732</v>
@@ -24411,10 +24411,10 @@
         <v>0.9038858049167328</v>
       </c>
       <c r="AQ24" t="n">
-        <v>1.021052631578947</v>
+        <v>0.9433955618175414</v>
       </c>
       <c r="AR24" t="n">
-        <v>1.021052631578947</v>
+        <v>0.9433955618175414</v>
       </c>
       <c r="AS24" t="n">
         <v>0.9865144830232112</v>
@@ -24518,10 +24518,10 @@
         <v>0.9257088396473672</v>
       </c>
       <c r="I25" t="n">
-        <v>1.019548872180451</v>
+        <v>0.9322296583303981</v>
       </c>
       <c r="J25" t="n">
-        <v>1.019548872180451</v>
+        <v>0.9322296583303981</v>
       </c>
       <c r="K25" t="n">
         <v>0.9923392052437525</v>
@@ -24620,10 +24620,10 @@
         <v>0.9043880518107322</v>
       </c>
       <c r="AQ25" t="n">
-        <v>1.019548872180451</v>
+        <v>0.9322296583303981</v>
       </c>
       <c r="AR25" t="n">
-        <v>1.019548872180451</v>
+        <v>0.9322296583303981</v>
       </c>
       <c r="AS25" t="n">
         <v>0.9924036063686936</v>
@@ -24727,10 +24727,10 @@
         <v>0.9272813914700976</v>
       </c>
       <c r="I26" t="n">
-        <v>1.018045112781955</v>
+        <v>0.9210637548432546</v>
       </c>
       <c r="J26" t="n">
-        <v>1.018045112781955</v>
+        <v>0.9210637548432546</v>
       </c>
       <c r="K26" t="n">
         <v>0.9982384268742319</v>
@@ -24829,10 +24829,10 @@
         <v>0.9048902987047317</v>
       </c>
       <c r="AQ26" t="n">
-        <v>1.018045112781955</v>
+        <v>0.9210637548432546</v>
       </c>
       <c r="AR26" t="n">
-        <v>1.018045112781955</v>
+        <v>0.9210637548432546</v>
       </c>
       <c r="AS26" t="n">
         <v>0.9982927297141762</v>
@@ -24936,10 +24936,10 @@
         <v>0.9288539432928281</v>
       </c>
       <c r="I27" t="n">
-        <v>1.016541353383459</v>
+        <v>0.9098978513561113</v>
       </c>
       <c r="J27" t="n">
-        <v>1.016541353383459</v>
+        <v>0.9098978513561113</v>
       </c>
       <c r="K27" t="n">
         <v>1.004137648504711</v>
@@ -25038,10 +25038,10 @@
         <v>0.9053925455987312</v>
       </c>
       <c r="AQ27" t="n">
-        <v>1.016541353383459</v>
+        <v>0.9098978513561113</v>
       </c>
       <c r="AR27" t="n">
-        <v>1.016541353383459</v>
+        <v>0.9098978513561113</v>
       </c>
       <c r="AS27" t="n">
         <v>1.004181853059658</v>
@@ -25145,10 +25145,10 @@
         <v>0.9304264951155586</v>
       </c>
       <c r="I28" t="n">
-        <v>1.015037593984963</v>
+        <v>0.8987319478689679</v>
       </c>
       <c r="J28" t="n">
-        <v>1.015037593984963</v>
+        <v>0.8987319478689679</v>
       </c>
       <c r="K28" t="n">
         <v>1.010036870135191</v>
@@ -25247,10 +25247,10 @@
         <v>0.9058947924927306</v>
       </c>
       <c r="AQ28" t="n">
-        <v>1.015037593984963</v>
+        <v>0.8987319478689679</v>
       </c>
       <c r="AR28" t="n">
-        <v>1.015037593984963</v>
+        <v>0.8987319478689679</v>
       </c>
       <c r="AS28" t="n">
         <v>1.010070976405141</v>
@@ -25354,10 +25354,10 @@
         <v>0.9350011913271383</v>
       </c>
       <c r="I29" t="n">
-        <v>1.014285714285714</v>
+        <v>0.8865445579429376</v>
       </c>
       <c r="J29" t="n">
-        <v>1.014285714285714</v>
+        <v>0.8865445579429376</v>
       </c>
       <c r="K29" t="n">
         <v>1.019377304383449</v>
@@ -25456,10 +25456,10 @@
         <v>0.9092783505154639</v>
       </c>
       <c r="AQ29" t="n">
-        <v>1.014285714285714</v>
+        <v>0.8865445579429376</v>
       </c>
       <c r="AR29" t="n">
-        <v>1.014285714285714</v>
+        <v>0.8865445579429376</v>
       </c>
       <c r="AS29" t="n">
         <v>1.019422597352772</v>
@@ -25563,10 +25563,10 @@
         <v>0.9395758875387181</v>
       </c>
       <c r="I30" t="n">
-        <v>1.013533834586466</v>
+        <v>0.8743571680169073</v>
       </c>
       <c r="J30" t="n">
-        <v>1.013533834586466</v>
+        <v>0.8743571680169073</v>
       </c>
       <c r="K30" t="n">
         <v>1.028717738631708</v>
@@ -25665,10 +25665,10 @@
         <v>0.9126619085381972</v>
       </c>
       <c r="AQ30" t="n">
-        <v>1.013533834586466</v>
+        <v>0.8743571680169073</v>
       </c>
       <c r="AR30" t="n">
-        <v>1.013533834586466</v>
+        <v>0.8743571680169073</v>
       </c>
       <c r="AS30" t="n">
         <v>1.028774218300403</v>
@@ -25772,10 +25772,10 @@
         <v>0.9441505837502978</v>
       </c>
       <c r="I31" t="n">
-        <v>1.012781954887218</v>
+        <v>0.8621697780908771</v>
       </c>
       <c r="J31" t="n">
-        <v>1.012781954887218</v>
+        <v>0.8621697780908771</v>
       </c>
       <c r="K31" t="n">
         <v>1.038058172879967</v>
@@ -25874,10 +25874,10 @@
         <v>0.9160454665609306</v>
       </c>
       <c r="AQ31" t="n">
-        <v>1.012781954887218</v>
+        <v>0.8621697780908771</v>
       </c>
       <c r="AR31" t="n">
-        <v>1.012781954887218</v>
+        <v>0.8621697780908771</v>
       </c>
       <c r="AS31" t="n">
         <v>1.038125839248034</v>
@@ -25981,10 +25981,10 @@
         <v>0.9487252799618776</v>
       </c>
       <c r="I32" t="n">
-        <v>1.01203007518797</v>
+        <v>0.8499823881648468</v>
       </c>
       <c r="J32" t="n">
-        <v>1.01203007518797</v>
+        <v>0.8499823881648468</v>
       </c>
       <c r="K32" t="n">
         <v>1.047398607128226</v>
@@ -26083,10 +26083,10 @@
         <v>0.9194290245836638</v>
       </c>
       <c r="AQ32" t="n">
-        <v>1.01203007518797</v>
+        <v>0.8499823881648468</v>
       </c>
       <c r="AR32" t="n">
-        <v>1.01203007518797</v>
+        <v>0.8499823881648468</v>
       </c>
       <c r="AS32" t="n">
         <v>1.047477460195664</v>
@@ -26190,10 +26190,10 @@
         <v>0.9532999761734573</v>
       </c>
       <c r="I33" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8377949982388165</v>
       </c>
       <c r="J33" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8377949982388165</v>
       </c>
       <c r="K33" t="n">
         <v>1.056739041376485</v>
@@ -26292,10 +26292,10 @@
         <v>0.9228125826063971</v>
       </c>
       <c r="AQ33" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8377949982388165</v>
       </c>
       <c r="AR33" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8377949982388165</v>
       </c>
       <c r="AS33" t="n">
         <v>1.056829081143295</v>
@@ -26399,10 +26399,10 @@
         <v>0.9579699785561115</v>
       </c>
       <c r="I34" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8264353645649877</v>
       </c>
       <c r="J34" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8264353645649877</v>
       </c>
       <c r="K34" t="n">
         <v>1.066509627201966</v>
@@ -26501,10 +26501,10 @@
         <v>0.9262754427702882</v>
       </c>
       <c r="AQ34" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8264353645649877</v>
       </c>
       <c r="AR34" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8264353645649877</v>
       </c>
       <c r="AS34" t="n">
         <v>1.066597928256282</v>
@@ -26608,10 +26608,10 @@
         <v>0.9626399809387658</v>
       </c>
       <c r="I35" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8150757308911589</v>
       </c>
       <c r="J35" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8150757308911589</v>
       </c>
       <c r="K35" t="n">
         <v>1.076280213027448</v>
@@ -26710,10 +26710,10 @@
         <v>0.9297383029341793</v>
       </c>
       <c r="AQ35" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8150757308911589</v>
       </c>
       <c r="AR35" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8150757308911589</v>
       </c>
       <c r="AS35" t="n">
         <v>1.076366775369269</v>
@@ -26817,10 +26817,10 @@
         <v>0.9673099833214202</v>
       </c>
       <c r="I36" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8037160972173301</v>
       </c>
       <c r="J36" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8037160972173301</v>
       </c>
       <c r="K36" t="n">
         <v>1.086050798852929</v>
@@ -26919,10 +26919,10 @@
         <v>0.9332011630980703</v>
       </c>
       <c r="AQ36" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8037160972173301</v>
       </c>
       <c r="AR36" t="n">
-        <v>1.011278195488722</v>
+        <v>0.8037160972173301</v>
       </c>
       <c r="AS36" t="n">
         <v>1.086135622482256</v>
@@ -27026,10 +27026,10 @@
         <v>0.9719799857040744</v>
       </c>
       <c r="I37" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7923564635435013</v>
       </c>
       <c r="J37" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7923564635435013</v>
       </c>
       <c r="K37" t="n">
         <v>1.095821384678411</v>
@@ -27128,10 +27128,10 @@
         <v>0.9366640232619614</v>
       </c>
       <c r="AQ37" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7923564635435013</v>
       </c>
       <c r="AR37" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7923564635435013</v>
       </c>
       <c r="AS37" t="n">
         <v>1.095904469595242</v>
@@ -27235,10 +27235,10 @@
         <v>0.9766499880867286</v>
       </c>
       <c r="I38" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7809968298696724</v>
       </c>
       <c r="J38" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7809968298696724</v>
       </c>
       <c r="K38" t="n">
         <v>1.105591970503892</v>
@@ -27337,10 +27337,10 @@
         <v>0.9401268834258525</v>
       </c>
       <c r="AQ38" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7809968298696724</v>
       </c>
       <c r="AR38" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7809968298696724</v>
       </c>
       <c r="AS38" t="n">
         <v>1.105673316708229</v>
@@ -27444,10 +27444,10 @@
         <v>0.9813199904693829</v>
       </c>
       <c r="I39" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7696371961958437</v>
       </c>
       <c r="J39" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7696371961958437</v>
       </c>
       <c r="K39" t="n">
         <v>1.115362556329373</v>
@@ -27546,10 +27546,10 @@
         <v>0.9435897435897437</v>
       </c>
       <c r="AQ39" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7696371961958437</v>
       </c>
       <c r="AR39" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7696371961958437</v>
       </c>
       <c r="AS39" t="n">
         <v>1.115442163821216</v>
@@ -27653,10 +27653,10 @@
         <v>0.9859899928520371</v>
       </c>
       <c r="I40" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7582775625220148</v>
       </c>
       <c r="J40" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7582775625220148</v>
       </c>
       <c r="K40" t="n">
         <v>1.125133142154855</v>
@@ -27755,10 +27755,10 @@
         <v>0.9470526037536348</v>
       </c>
       <c r="AQ40" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7582775625220148</v>
       </c>
       <c r="AR40" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7582775625220148</v>
       </c>
       <c r="AS40" t="n">
         <v>1.125211010934203</v>
@@ -27862,10 +27862,10 @@
         <v>0.9906599952346915</v>
       </c>
       <c r="I41" t="n">
-        <v>1.011278195488722</v>
+        <v>0.746917928848186</v>
       </c>
       <c r="J41" t="n">
-        <v>1.011278195488722</v>
+        <v>0.746917928848186</v>
       </c>
       <c r="K41" t="n">
         <v>1.134903727980336</v>
@@ -27964,10 +27964,10 @@
         <v>0.9505154639175258</v>
       </c>
       <c r="AQ41" t="n">
-        <v>1.011278195488722</v>
+        <v>0.746917928848186</v>
       </c>
       <c r="AR41" t="n">
-        <v>1.011278195488722</v>
+        <v>0.746917928848186</v>
       </c>
       <c r="AS41" t="n">
         <v>1.13497985804719</v>
@@ -28071,10 +28071,10 @@
         <v>0.9953299976173458</v>
       </c>
       <c r="I42" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7355582951743572</v>
       </c>
       <c r="J42" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7355582951743572</v>
       </c>
       <c r="K42" t="n">
         <v>1.144674313805818</v>
@@ -28173,10 +28173,10 @@
         <v>0.9539783240814169</v>
       </c>
       <c r="AQ42" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7355582951743572</v>
       </c>
       <c r="AR42" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7355582951743572</v>
       </c>
       <c r="AS42" t="n">
         <v>1.144748705160176</v>
@@ -28280,10 +28280,10 @@
         <v>1</v>
       </c>
       <c r="I43" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7241986615005284</v>
       </c>
       <c r="J43" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7241986615005284</v>
       </c>
       <c r="K43" t="n">
         <v>1.154444899631299</v>
@@ -28382,10 +28382,10 @@
         <v>0.957441184245308</v>
       </c>
       <c r="AQ43" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7241986615005284</v>
       </c>
       <c r="AR43" t="n">
-        <v>1.011278195488722</v>
+        <v>0.7241986615005284</v>
       </c>
       <c r="AS43" t="n">
         <v>1.154517552273163</v>

</xml_diff>